<commit_message>
initial VS mov & no depth opt experiments
</commit_message>
<xml_diff>
--- a/Data/Excels/Resumes/Depth - Experiment 1.xlsx
+++ b/Data/Excels/Resumes/Depth - Experiment 1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:AE11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,52 +466,127 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>ARAP-InRays Initial VS Mov (%)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>ARAP-TwoPoints Improvement (%)</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>ARAP-TwoPoints Final Vs Mov (%)</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>ARAP-TwoPoints Initial VS Mov (%)</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>ARAP-FarPoints Improvement (%)</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>ARAP-FarPoints Final Vs Mov (%)</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>ARAP-FarPoints Initial VS Mov (%)</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>ARAP_depth-InRays Improvement (%)</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>ARAP_depth-InRays Final Vs Mov (%)</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>ARAP_depth-InRays Initial VS Mov (%)</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>ARAP_depth-TwoPoints Improvement (%)</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>ARAP_depth-TwoPoints Final Vs Mov (%)</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>ARAP_depth-TwoPoints Initial VS Mov (%)</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>ARAP_depth-FarPoints Improvement (%)</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>ARAP_depth-FarPoints Final Vs Mov (%)</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>ARAP_depth-FarPoints Initial VS Mov (%)</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>ARAP_depth_onlyTriang-InRays Improvement (%)</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>ARAP_depth_onlyTriang-InRays Final Vs Mov (%)</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>ARAP_depth_onlyTriang-InRays Initial VS Mov (%)</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>ARAP_depth_onlyTriang-TwoPoints Improvement (%)</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>ARAP_depth_onlyTriang-TwoPoints Final Vs Mov (%)</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>ARAP_depth_onlyTriang-TwoPoints Initial VS Mov (%)</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>ARAP_depth_onlyTriang-FarPoints Improvement (%)</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>ARAP_depth_onlyTriang-FarPoints Final Vs Mov (%)</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>ARAP_depth_onlyTriang-FarPoints Initial VS Mov (%)</t>
         </is>
       </c>
     </row>
@@ -537,34 +612,79 @@
         <v>83.23</v>
       </c>
       <c r="G2" t="n">
+        <v>77.97</v>
+      </c>
+      <c r="H2" t="n">
         <v>4.25</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>81.78</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
+        <v>85.31999999999999</v>
+      </c>
+      <c r="K2" t="n">
         <v>-5.87</v>
       </c>
-      <c r="J2" t="n">
+      <c r="L2" t="n">
         <v>91.40000000000001</v>
       </c>
-      <c r="K2" t="n">
+      <c r="M2" t="n">
+        <v>86.33</v>
+      </c>
+      <c r="N2" t="n">
         <v>-204.5</v>
       </c>
-      <c r="L2" t="n">
+      <c r="O2" t="n">
         <v>82.81999999999999</v>
       </c>
-      <c r="M2" t="n">
+      <c r="P2" t="n">
+        <v>27.09</v>
+      </c>
+      <c r="Q2" t="n">
         <v>-47.81</v>
       </c>
-      <c r="N2" t="n">
+      <c r="R2" t="n">
         <v>80.34999999999999</v>
       </c>
-      <c r="O2" t="n">
+      <c r="S2" t="n">
+        <v>54.43</v>
+      </c>
+      <c r="T2" t="n">
         <v>-52.51</v>
       </c>
-      <c r="P2" t="n">
+      <c r="U2" t="n">
         <v>100.95</v>
+      </c>
+      <c r="V2" t="n">
+        <v>66.08</v>
+      </c>
+      <c r="W2" t="n">
+        <v>-207.24</v>
+      </c>
+      <c r="X2" t="n">
+        <v>83.56</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>27.09</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>-44.02</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>78.29000000000001</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>54.43</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>-53.05</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>101.3</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>66.08</v>
       </c>
     </row>
     <row r="3">
@@ -583,40 +703,85 @@
         <v>2.5</v>
       </c>
       <c r="E3" t="n">
-        <v>-6.74</v>
+        <v>6.28</v>
       </c>
       <c r="F3" t="n">
-        <v>83.23</v>
+        <v>56.77</v>
       </c>
       <c r="G3" t="n">
-        <v>4.25</v>
+        <v>60.4</v>
       </c>
       <c r="H3" t="n">
-        <v>81.78</v>
+        <v>11.46</v>
       </c>
       <c r="I3" t="n">
-        <v>-5.87</v>
+        <v>58.18</v>
       </c>
       <c r="J3" t="n">
-        <v>91.40000000000001</v>
+        <v>65.59999999999999</v>
       </c>
       <c r="K3" t="n">
-        <v>-204.5</v>
+        <v>24.38</v>
       </c>
       <c r="L3" t="n">
-        <v>82.81999999999999</v>
+        <v>53.45</v>
       </c>
       <c r="M3" t="n">
-        <v>-47.81</v>
+        <v>70.8</v>
       </c>
       <c r="N3" t="n">
-        <v>80.34999999999999</v>
+        <v>23.31</v>
       </c>
       <c r="O3" t="n">
-        <v>-52.51</v>
+        <v>32.9</v>
       </c>
       <c r="P3" t="n">
-        <v>100.95</v>
+        <v>42.8</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>28.37</v>
+      </c>
+      <c r="R3" t="n">
+        <v>40.69</v>
+      </c>
+      <c r="S3" t="n">
+        <v>56.8</v>
+      </c>
+      <c r="T3" t="n">
+        <v>55.51</v>
+      </c>
+      <c r="U3" t="n">
+        <v>37.2</v>
+      </c>
+      <c r="V3" t="n">
+        <v>83.59999999999999</v>
+      </c>
+      <c r="W3" t="n">
+        <v>23.82</v>
+      </c>
+      <c r="X3" t="n">
+        <v>32.68</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>42.8</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>28.47</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>40.63</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>56.8</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>55.47</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>37.23</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>83.59999999999999</v>
       </c>
     </row>
     <row r="4">
@@ -635,40 +800,85 @@
         <v>2.5</v>
       </c>
       <c r="E4" t="n">
-        <v>-6.74</v>
+        <v>-1.78</v>
       </c>
       <c r="F4" t="n">
-        <v>83.23</v>
+        <v>68.26000000000001</v>
       </c>
       <c r="G4" t="n">
-        <v>4.25</v>
+        <v>67.02</v>
       </c>
       <c r="H4" t="n">
-        <v>81.78</v>
+        <v>7.44</v>
       </c>
       <c r="I4" t="n">
-        <v>-5.87</v>
+        <v>68.36</v>
       </c>
       <c r="J4" t="n">
-        <v>91.40000000000001</v>
+        <v>73.78</v>
       </c>
       <c r="K4" t="n">
-        <v>-204.5</v>
+        <v>12.15</v>
       </c>
       <c r="L4" t="n">
-        <v>82.81999999999999</v>
+        <v>66.38</v>
       </c>
       <c r="M4" t="n">
-        <v>-47.81</v>
+        <v>75.48</v>
       </c>
       <c r="N4" t="n">
-        <v>80.34999999999999</v>
+        <v>-178.72</v>
       </c>
       <c r="O4" t="n">
-        <v>-52.51</v>
+        <v>63.8</v>
       </c>
       <c r="P4" t="n">
-        <v>100.95</v>
+        <v>22.83</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>-20.02</v>
+      </c>
+      <c r="R4" t="n">
+        <v>63.65</v>
+      </c>
+      <c r="S4" t="n">
+        <v>53.07</v>
+      </c>
+      <c r="T4" t="n">
+        <v>-70.81999999999999</v>
+      </c>
+      <c r="U4" t="n">
+        <v>109.69</v>
+      </c>
+      <c r="V4" t="n">
+        <v>64.06</v>
+      </c>
+      <c r="W4" t="n">
+        <v>-177.44</v>
+      </c>
+      <c r="X4" t="n">
+        <v>63.51</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>22.83</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>-19.08</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>63.15</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>53.07</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>-71.23999999999999</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>109.95</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>64.06</v>
       </c>
     </row>
     <row r="5">
@@ -687,40 +897,85 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>-6.74</v>
+        <v>-6.16</v>
       </c>
       <c r="F5" t="n">
-        <v>83.23</v>
+        <v>80.90000000000001</v>
       </c>
       <c r="G5" t="n">
-        <v>4.25</v>
+        <v>76.26000000000001</v>
       </c>
       <c r="H5" t="n">
-        <v>81.78</v>
+        <v>5.95</v>
       </c>
       <c r="I5" t="n">
-        <v>-5.87</v>
+        <v>80.68000000000001</v>
       </c>
       <c r="J5" t="n">
-        <v>91.40000000000001</v>
+        <v>85.79000000000001</v>
       </c>
       <c r="K5" t="n">
-        <v>-204.5</v>
+        <v>1.63</v>
       </c>
       <c r="L5" t="n">
-        <v>82.81999999999999</v>
+        <v>84.69</v>
       </c>
       <c r="M5" t="n">
-        <v>-47.81</v>
+        <v>86.11</v>
       </c>
       <c r="N5" t="n">
-        <v>80.34999999999999</v>
+        <v>-1648.69</v>
       </c>
       <c r="O5" t="n">
-        <v>-52.51</v>
+        <v>116.83</v>
       </c>
       <c r="P5" t="n">
-        <v>100.95</v>
+        <v>6.67</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>-121.04</v>
+      </c>
+      <c r="R5" t="n">
+        <v>111.01</v>
+      </c>
+      <c r="S5" t="n">
+        <v>50.22</v>
+      </c>
+      <c r="T5" t="n">
+        <v>-1603.6</v>
+      </c>
+      <c r="U5" t="n">
+        <v>873.0700000000001</v>
+      </c>
+      <c r="V5" t="n">
+        <v>51.28</v>
+      </c>
+      <c r="W5" t="n">
+        <v>-1753.71</v>
+      </c>
+      <c r="X5" t="n">
+        <v>123.85</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>6.67</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>-106.49</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>103.7</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>50.22</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>-1598.78</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>870.59</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>51.28</v>
       </c>
     </row>
     <row r="6">
@@ -739,40 +994,85 @@
         <v>10</v>
       </c>
       <c r="E6" t="n">
-        <v>-6.74</v>
+        <v>5.15</v>
       </c>
       <c r="F6" t="n">
-        <v>83.23</v>
+        <v>44.11</v>
       </c>
       <c r="G6" t="n">
-        <v>4.25</v>
+        <v>46.5</v>
       </c>
       <c r="H6" t="n">
-        <v>81.78</v>
+        <v>18.19</v>
       </c>
       <c r="I6" t="n">
-        <v>-5.87</v>
+        <v>45.57</v>
       </c>
       <c r="J6" t="n">
-        <v>91.40000000000001</v>
+        <v>55.7</v>
       </c>
       <c r="K6" t="n">
-        <v>-204.5</v>
+        <v>34.95</v>
       </c>
       <c r="L6" t="n">
-        <v>82.81999999999999</v>
+        <v>36.55</v>
       </c>
       <c r="M6" t="n">
-        <v>-47.81</v>
+        <v>56.2</v>
       </c>
       <c r="N6" t="n">
-        <v>80.34999999999999</v>
+        <v>23.21</v>
       </c>
       <c r="O6" t="n">
-        <v>-52.51</v>
+        <v>8.08</v>
       </c>
       <c r="P6" t="n">
-        <v>100.95</v>
+        <v>10.5</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>80.31</v>
+      </c>
+      <c r="R6" t="n">
+        <v>9.92</v>
+      </c>
+      <c r="S6" t="n">
+        <v>50.4</v>
+      </c>
+      <c r="T6" t="n">
+        <v>57.33</v>
+      </c>
+      <c r="U6" t="n">
+        <v>22.48</v>
+      </c>
+      <c r="V6" t="n">
+        <v>52.7</v>
+      </c>
+      <c r="W6" t="n">
+        <v>22.98</v>
+      </c>
+      <c r="X6" t="n">
+        <v>8.109999999999999</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>54.02</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>23.16</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>50.4</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>57.6</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>22.34</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>52.7</v>
       </c>
     </row>
     <row r="7">
@@ -791,40 +1091,85 @@
         <v>10</v>
       </c>
       <c r="E7" t="n">
-        <v>-6.74</v>
+        <v>-2.05</v>
       </c>
       <c r="F7" t="n">
-        <v>83.23</v>
+        <v>68.78</v>
       </c>
       <c r="G7" t="n">
-        <v>4.25</v>
+        <v>67.40000000000001</v>
       </c>
       <c r="H7" t="n">
-        <v>81.78</v>
+        <v>9.68</v>
       </c>
       <c r="I7" t="n">
-        <v>-5.87</v>
+        <v>68.83</v>
       </c>
       <c r="J7" t="n">
-        <v>91.40000000000001</v>
+        <v>76.23</v>
       </c>
       <c r="K7" t="n">
-        <v>-204.5</v>
+        <v>-54.31</v>
       </c>
       <c r="L7" t="n">
-        <v>82.81999999999999</v>
+        <v>117.73</v>
       </c>
       <c r="M7" t="n">
-        <v>-47.81</v>
+        <v>76.28</v>
       </c>
       <c r="N7" t="n">
-        <v>80.34999999999999</v>
+        <v>-5558.03</v>
       </c>
       <c r="O7" t="n">
-        <v>-52.51</v>
+        <v>311</v>
       </c>
       <c r="P7" t="n">
-        <v>100.95</v>
+        <v>5.49</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>-70.43000000000001</v>
+      </c>
+      <c r="R7" t="n">
+        <v>85.48999999999999</v>
+      </c>
+      <c r="S7" t="n">
+        <v>50.16</v>
+      </c>
+      <c r="T7" t="n">
+        <v>-1042.32</v>
+      </c>
+      <c r="U7" t="n">
+        <v>577.89</v>
+      </c>
+      <c r="V7" t="n">
+        <v>50.57</v>
+      </c>
+      <c r="W7" t="n">
+        <v>-5574.19</v>
+      </c>
+      <c r="X7" t="n">
+        <v>311.89</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>5.49</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>-68.58</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>84.56</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>50.16</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>-1066.05</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>589.9</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>50.57</v>
       </c>
     </row>
     <row r="8">
@@ -843,40 +1188,85 @@
         <v>2.5</v>
       </c>
       <c r="E8" t="n">
-        <v>-6.74</v>
+        <v>-0.45</v>
       </c>
       <c r="F8" t="n">
-        <v>83.23</v>
+        <v>53.76</v>
       </c>
       <c r="G8" t="n">
-        <v>4.25</v>
+        <v>53.4</v>
       </c>
       <c r="H8" t="n">
-        <v>81.78</v>
+        <v>14.46</v>
       </c>
       <c r="I8" t="n">
-        <v>-5.87</v>
+        <v>53.61</v>
       </c>
       <c r="J8" t="n">
-        <v>91.40000000000001</v>
+        <v>62.65</v>
       </c>
       <c r="K8" t="n">
-        <v>-204.5</v>
+        <v>40.69</v>
       </c>
       <c r="L8" t="n">
-        <v>82.81999999999999</v>
+        <v>39.56</v>
       </c>
       <c r="M8" t="n">
-        <v>-47.81</v>
+        <v>66.67</v>
       </c>
       <c r="N8" t="n">
-        <v>80.34999999999999</v>
+        <v>-25.48</v>
       </c>
       <c r="O8" t="n">
-        <v>-52.51</v>
+        <v>41.36</v>
       </c>
       <c r="P8" t="n">
-        <v>100.95</v>
+        <v>33.02</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>30.17</v>
+      </c>
+      <c r="R8" t="n">
+        <v>39.67</v>
+      </c>
+      <c r="S8" t="n">
+        <v>56.79</v>
+      </c>
+      <c r="T8" t="n">
+        <v>47.24</v>
+      </c>
+      <c r="U8" t="n">
+        <v>39.62</v>
+      </c>
+      <c r="V8" t="n">
+        <v>75</v>
+      </c>
+      <c r="W8" t="n">
+        <v>-25.84</v>
+      </c>
+      <c r="X8" t="n">
+        <v>41.48</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>33.02</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>29.88</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>39.83</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>56.79</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>47.23</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>39.63</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>75</v>
       </c>
     </row>
     <row r="9">
@@ -895,40 +1285,85 @@
         <v>2.5</v>
       </c>
       <c r="E9" t="n">
-        <v>-6.74</v>
+        <v>-2.38</v>
       </c>
       <c r="F9" t="n">
-        <v>83.23</v>
+        <v>68.70999999999999</v>
       </c>
       <c r="G9" t="n">
-        <v>4.25</v>
+        <v>66.98</v>
       </c>
       <c r="H9" t="n">
-        <v>81.78</v>
+        <v>8.130000000000001</v>
       </c>
       <c r="I9" t="n">
-        <v>-5.87</v>
+        <v>69.17</v>
       </c>
       <c r="J9" t="n">
-        <v>91.40000000000001</v>
+        <v>75.19</v>
       </c>
       <c r="K9" t="n">
-        <v>-204.5</v>
+        <v>11.83</v>
       </c>
       <c r="L9" t="n">
-        <v>82.81999999999999</v>
+        <v>67.13</v>
       </c>
       <c r="M9" t="n">
-        <v>-47.81</v>
+        <v>76.12</v>
       </c>
       <c r="N9" t="n">
-        <v>80.34999999999999</v>
+        <v>-279.55</v>
       </c>
       <c r="O9" t="n">
-        <v>-52.51</v>
+        <v>74.98</v>
       </c>
       <c r="P9" t="n">
-        <v>100.95</v>
+        <v>19.78</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>-28.81</v>
+      </c>
+      <c r="R9" t="n">
+        <v>67.06999999999999</v>
+      </c>
+      <c r="S9" t="n">
+        <v>52.05</v>
+      </c>
+      <c r="T9" t="n">
+        <v>-25.81</v>
+      </c>
+      <c r="U9" t="n">
+        <v>75.98</v>
+      </c>
+      <c r="V9" t="n">
+        <v>60.26</v>
+      </c>
+      <c r="W9" t="n">
+        <v>-276.27</v>
+      </c>
+      <c r="X9" t="n">
+        <v>74.33</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>19.78</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>-27.46</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>66.37</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>52.05</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>-28.46</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>77.58</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>60.26</v>
       </c>
     </row>
     <row r="10">
@@ -947,40 +1382,85 @@
         <v>10</v>
       </c>
       <c r="E10" t="n">
-        <v>-6.74</v>
+        <v>45.75</v>
       </c>
       <c r="F10" t="n">
-        <v>83.23</v>
+        <v>23.82</v>
       </c>
       <c r="G10" t="n">
-        <v>4.25</v>
+        <v>43.87</v>
       </c>
       <c r="H10" t="n">
-        <v>81.78</v>
+        <v>39.17</v>
       </c>
       <c r="I10" t="n">
-        <v>-5.87</v>
+        <v>33.6</v>
       </c>
       <c r="J10" t="n">
-        <v>91.40000000000001</v>
+        <v>55.27</v>
       </c>
       <c r="K10" t="n">
-        <v>-204.5</v>
+        <v>44.44</v>
       </c>
       <c r="L10" t="n">
-        <v>82.81999999999999</v>
+        <v>30.91</v>
       </c>
       <c r="M10" t="n">
-        <v>-47.81</v>
+        <v>55.65</v>
       </c>
       <c r="N10" t="n">
-        <v>80.34999999999999</v>
+        <v>-113.74</v>
       </c>
       <c r="O10" t="n">
-        <v>-52.51</v>
+        <v>21.16</v>
       </c>
       <c r="P10" t="n">
-        <v>100.95</v>
+        <v>9.880000000000001</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>53.37</v>
+      </c>
+      <c r="R10" t="n">
+        <v>23.72</v>
+      </c>
+      <c r="S10" t="n">
+        <v>50.9</v>
+      </c>
+      <c r="T10" t="n">
+        <v>68.61</v>
+      </c>
+      <c r="U10" t="n">
+        <v>16.9</v>
+      </c>
+      <c r="V10" t="n">
+        <v>53.85</v>
+      </c>
+      <c r="W10" t="n">
+        <v>-113.62</v>
+      </c>
+      <c r="X10" t="n">
+        <v>21.15</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>9.880000000000001</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>55.97</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>22.39</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>50.9</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>68.40000000000001</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>17.02</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>53.85</v>
       </c>
     </row>
     <row r="11">
@@ -999,40 +1479,85 @@
         <v>10</v>
       </c>
       <c r="E11" t="n">
-        <v>-6.74</v>
+        <v>-4.99</v>
       </c>
       <c r="F11" t="n">
-        <v>83.23</v>
+        <v>67.73</v>
       </c>
       <c r="G11" t="n">
-        <v>4.25</v>
+        <v>64.52</v>
       </c>
       <c r="H11" t="n">
-        <v>81.78</v>
+        <v>10.76</v>
       </c>
       <c r="I11" t="n">
-        <v>-5.87</v>
+        <v>67.38</v>
       </c>
       <c r="J11" t="n">
-        <v>91.40000000000001</v>
+        <v>75.48</v>
       </c>
       <c r="K11" t="n">
-        <v>-204.5</v>
+        <v>-5.8</v>
       </c>
       <c r="L11" t="n">
-        <v>82.81999999999999</v>
+        <v>79.65000000000001</v>
       </c>
       <c r="M11" t="n">
-        <v>-47.81</v>
+        <v>75.27</v>
       </c>
       <c r="N11" t="n">
-        <v>80.34999999999999</v>
+        <v>-10788.04</v>
       </c>
       <c r="O11" t="n">
-        <v>-52.51</v>
+        <v>585.6</v>
       </c>
       <c r="P11" t="n">
-        <v>100.95</v>
+        <v>5.4</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>-64.11</v>
+      </c>
+      <c r="R11" t="n">
+        <v>82.36</v>
+      </c>
+      <c r="S11" t="n">
+        <v>50.18</v>
+      </c>
+      <c r="T11" t="n">
+        <v>-1066.75</v>
+      </c>
+      <c r="U11" t="n">
+        <v>589.77</v>
+      </c>
+      <c r="V11" t="n">
+        <v>50.54</v>
+      </c>
+      <c r="W11" t="n">
+        <v>-10821.31</v>
+      </c>
+      <c r="X11" t="n">
+        <v>587.39</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>-68.70999999999999</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>84.67</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>50.18</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>-1067.6</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>590.1900000000001</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>50.54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>